<commit_message>
finished afcea nova, starting afcea dc
</commit_message>
<xml_diff>
--- a/act-iac/ACT-IAC_Events-03.06.23.xlsx
+++ b/act-iac/ACT-IAC_Events-03.06.23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorcas/Development/python_scraper_parser_projects/act-iac/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7C3670-DEFF-8B44-AA8C-7DDA856B0258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A43356-BDD8-C644-BFCB-3AE9D7F6A513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events Calendar" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="173">
   <si>
     <t>Event Type</t>
   </si>
@@ -423,9 +423,6 @@
     <t>https://www.actiac.org/project-activity/ato-code</t>
   </si>
   <si>
-    <t>https://www.actiac.org/events/act-iac-emerging-technology-coi-november-2019</t>
-  </si>
-  <si>
     <t>https://www.actiac.org/project-activity/blockchain-and-distributed-ledger-technology-project</t>
   </si>
   <si>
@@ -442,6 +439,108 @@
   </si>
   <si>
     <t>https://www.actiac.org/project-activity/va-data-initiatives-and-priorities</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Brendan, Caroline</t>
+  </si>
+  <si>
+    <t>Gary Smith</t>
+  </si>
+  <si>
+    <t>Joe, Madeline St. Claire</t>
+  </si>
+  <si>
+    <t>Chris Burns</t>
+  </si>
+  <si>
+    <t>Joe, Caroline, Tatanya</t>
+  </si>
+  <si>
+    <t>*Might sponsor</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Dusti Patterson</t>
+  </si>
+  <si>
+    <t>Ian Kramer, Jamyi Light, Sarah Newton</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Emailed Madeline &amp; Joe, Joe C registered</t>
+  </si>
+  <si>
+    <t>Emailed Madeline, Joe C registered</t>
+  </si>
+  <si>
+    <t>Emailed Brendan, Joe C registered</t>
+  </si>
+  <si>
+    <t>Joe C, Jin Lim</t>
+  </si>
+  <si>
+    <t>Joe C, Madeline St. Claire</t>
+  </si>
+  <si>
+    <t>Joe C, Brendan McCann</t>
+  </si>
+  <si>
+    <t>Emailed Chris</t>
+  </si>
+  <si>
+    <t>*Might sponsor, Joe C on planning committee</t>
+  </si>
+  <si>
+    <t>Joe C and Erin L on planning committee</t>
+  </si>
+  <si>
+    <t>Joe C, Erin L</t>
+  </si>
+  <si>
+    <t>*Note: Grayed out items are one of less importance to SAS Fed team</t>
+  </si>
+  <si>
+    <t>Email sent to Ian, Jamyi, and Sarah</t>
+  </si>
+  <si>
+    <t>Message sent to Dusti</t>
+  </si>
+  <si>
+    <t>Joe Nash</t>
+  </si>
+  <si>
+    <t>Emailed Joe N</t>
+  </si>
+  <si>
+    <t>No lead for project</t>
+  </si>
+  <si>
+    <t>Active group - need to assign resource</t>
+  </si>
+  <si>
+    <t>Brendan McCann</t>
+  </si>
+  <si>
+    <t>Joe C and Madeline St. Claire attended; sent to Jin Lim late</t>
+  </si>
+  <si>
+    <t>Gary to attend, Joe has a customer conflict</t>
+  </si>
+  <si>
+    <t>Tatanya Szeglia, David Hendrie, Rob Wetzel</t>
+  </si>
+  <si>
+    <t>Emailed Tatanya, David, and Rob</t>
   </si>
 </sst>
 </file>
@@ -472,12 +571,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -496,7 +607,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -506,6 +617,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -845,10 +967,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -859,9 +982,10 @@
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79" style="4" customWidth="1"/>
     <col min="6" max="6" width="95.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,88 +1004,103 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="G3" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -977,11 +1116,17 @@
       <c r="E6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -994,8 +1139,14 @@
       <c r="F7" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1014,8 +1165,14 @@
       <c r="F8" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1031,31 +1188,37 @@
       <c r="E9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1071,8 +1234,14 @@
       <c r="F11" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>155</v>
+      </c>
+      <c r="H11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1091,25 +1260,32 @@
       <c r="F12" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1125,8 +1301,14 @@
       <c r="F14" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1145,8 +1327,11 @@
       <c r="F15" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1165,8 +1350,11 @@
       <c r="F16" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1179,8 +1367,14 @@
       <c r="F17" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1199,8 +1393,11 @@
       <c r="F18" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1216,8 +1413,14 @@
       <c r="F19" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1232,6 +1435,17 @@
       </c>
       <c r="F20" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="G20" t="s">
+        <v>146</v>
+      </c>
+      <c r="H20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1390,159 +1604,228 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>119</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>121</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>122</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>124</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>126</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>127</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>128</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
-        <v>139</v>
+      <c r="C21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1555,13 +1838,12 @@
     <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
     <hyperlink ref="B14" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
     <hyperlink ref="B15" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="B17" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="B18" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="B19" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="B20" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="B21" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="B22" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B19" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B20" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B21" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>